<commit_message>
Selected 8 user stories
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02786040-BBE3-4AAF-B682-4415C54CCFC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BC0D2D-14C2-487C-A14B-3B0C15267C8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3274,8 +3274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3350,14 +3350,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="35" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3537,14 +3537,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="37" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added selected stories in backlog tab and assigned to sprint1
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/Rahul/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Stevens\SSW555\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA76CE66-69E5-AB48-BFD7-CEE868A9D4C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70634FD-C0D5-46F2-A283-62F7F779F2C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$E$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$C$43</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="205">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -655,18 +659,12 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>NO Backlog yet</t>
-  </si>
-  <si>
     <t>Assigned</t>
   </si>
   <si>
     <t>Completed date</t>
   </si>
   <si>
-    <t>Not planned</t>
-  </si>
-  <si>
     <t>dpate111@stevens.edu</t>
   </si>
   <si>
@@ -686,6 +684,12 @@
   </si>
   <si>
     <t>anurag-aman</t>
+  </si>
+  <si>
+    <t>Not Planned</t>
+  </si>
+  <si>
+    <t>Planned</t>
   </si>
 </sst>
 </file>
@@ -696,7 +700,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -705,26 +709,31 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -743,6 +752,11 @@
       <color theme="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -860,7 +874,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -923,6 +937,7 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -992,7 +1007,16 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BBB59"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1032,7 +1056,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1103,7 +1127,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2086,20 +2110,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="14" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="14" customWidth="1"/>
     <col min="6" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -2116,9 +2140,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>179</v>
@@ -2133,9 +2157,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>181</v>
@@ -2147,12 +2171,12 @@
         <v>188</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.15">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>183</v>
@@ -2167,9 +2191,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>185</v>
@@ -2178,18 +2202,18 @@
         <v>186</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E5" s="30" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2210,23 +2234,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="14" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="14" customWidth="1"/>
+    <col min="1" max="2" width="6.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
@@ -2243,18 +2266,354 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="C3" s="16"/>
+      <c r="B2" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>203</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E25" xr:uid="{CF9EA074-D5DE-4C85-83F4-BAF6F52AE4EF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
+      <sortCondition ref="A1:A25"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2269,47 +2628,47 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="6"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>164</v>
       </c>
@@ -2332,7 +2691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -2348,7 +2707,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -2373,7 +2732,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>167</v>
       </c>
@@ -2398,7 +2757,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>168</v>
       </c>
@@ -2423,7 +2782,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>169</v>
       </c>
@@ -2463,16 +2822,16 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2492,7 +2851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>42633</v>
       </c>
@@ -2506,7 +2865,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>42657</v>
       </c>
@@ -2516,7 +2875,7 @@
       <c r="E3" s="14"/>
       <c r="F3" s="20"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
         <v>42683</v>
       </c>
@@ -2526,7 +2885,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="20"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>42708</v>
       </c>
@@ -2536,7 +2895,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="20"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>42728</v>
       </c>
@@ -2558,25 +2917,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="14" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="16" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="14" customWidth="1"/>
     <col min="4" max="4" width="11" style="14"/>
-    <col min="5" max="5" width="6.83203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="14" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="14" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
@@ -2602,27 +2961,27 @@
         <v>16</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E2" s="14">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="F2" s="14">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>193</v>
@@ -2634,24 +2993,24 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E3" s="14">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="F3" s="14">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>193</v>
@@ -2663,12 +3022,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>193</v>
@@ -2680,12 +3039,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>193</v>
@@ -2697,12 +3056,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C6" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>193</v>
@@ -2714,12 +3073,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C7" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>193</v>
@@ -2731,12 +3090,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>193</v>
@@ -2748,12 +3107,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C9" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>193</v>
@@ -2765,35 +3124,35 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
     </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B21" s="16" t="s">
         <v>36</v>
       </c>
@@ -2810,12 +3169,12 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
@@ -2844,128 +3203,88 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>197</v>
-      </c>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>197</v>
-      </c>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
-      <c r="C4" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -2984,12 +3303,12 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -3018,128 +3337,88 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>197</v>
-      </c>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>197</v>
-      </c>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
-      <c r="C4" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>197</v>
-      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -3154,18 +3433,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -3192,82 +3471,6 @@
       </c>
       <c r="I1" s="22" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C4" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C5" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C6" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C7" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C8" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C9" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -3278,19 +3481,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A5" sqref="A5:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>116</v>
       </c>
@@ -3301,7 +3505,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="38" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>117</v>
       </c>
@@ -3312,7 +3516,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" s="38" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>118</v>
       </c>
@@ -3323,7 +3527,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" s="38" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>119</v>
       </c>
@@ -3334,7 +3538,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>120</v>
       </c>
@@ -3345,7 +3549,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>121</v>
       </c>
@@ -3356,7 +3560,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>122</v>
       </c>
@@ -3367,7 +3571,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="38" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" s="38" customFormat="1" ht="47.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>123</v>
       </c>
@@ -3378,7 +3582,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -3389,7 +3593,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -3400,7 +3604,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -3411,7 +3615,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -3422,7 +3626,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="47.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -3433,7 +3637,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="63" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -3444,7 +3648,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>130</v>
       </c>
@@ -3455,7 +3659,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>131</v>
       </c>
@@ -3466,7 +3670,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>132</v>
       </c>
@@ -3477,7 +3681,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" s="38" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>133</v>
       </c>
@@ -3488,7 +3692,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -3499,7 +3703,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>135</v>
       </c>
@@ -3510,7 +3714,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -3521,7 +3725,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="38" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>137</v>
       </c>
@@ -3532,7 +3736,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -3543,7 +3747,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>139</v>
       </c>
@@ -3554,7 +3758,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="47.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -3565,7 +3769,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="38" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
         <v>141</v>
       </c>
@@ -3576,7 +3780,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="126" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>142</v>
       </c>
@@ -3587,7 +3791,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
         <v>143</v>
       </c>
@@ -3598,7 +3802,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>144</v>
       </c>
@@ -3609,7 +3813,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" s="32" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>145</v>
       </c>
@@ -3620,7 +3824,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" s="32" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>146</v>
       </c>
@@ -3631,7 +3835,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>147</v>
       </c>
@@ -3642,7 +3846,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" s="34" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
         <v>148</v>
       </c>
@@ -3653,7 +3857,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>149</v>
       </c>
@@ -3664,7 +3868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>150</v>
       </c>
@@ -3675,7 +3879,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>151</v>
       </c>
@@ -3686,7 +3890,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>152</v>
       </c>
@@ -3697,7 +3901,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -3708,7 +3912,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>154</v>
       </c>
@@ -3719,7 +3923,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -3730,7 +3934,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>156</v>
       </c>
@@ -3741,7 +3945,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>157</v>
       </c>
@@ -3752,7 +3956,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -3764,6 +3968,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C43" xr:uid="{FB908553-6618-4CAE-8A24-8792C31B8736}">
+    <filterColumn colId="2">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
Alternate program to process the GEDCOM file. Removed filter from stories tab
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Stevens\SSW555\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70634FD-C0D5-46F2-A283-62F7F779F2C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F2C564-EAB1-4190-ABC5-45E07C3FAADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2917,7 +2917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3481,11 +3481,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B41"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3505,7 +3504,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>117</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="38" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>118</v>
       </c>
@@ -3527,7 +3526,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="38" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>119</v>
       </c>
@@ -3560,7 +3559,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>122</v>
       </c>
@@ -3571,7 +3570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="38" customFormat="1" ht="47.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="38" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>123</v>
       </c>
@@ -3582,7 +3581,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -3593,7 +3592,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -3604,7 +3603,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -3615,7 +3614,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -3626,7 +3625,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -3637,7 +3636,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -3648,7 +3647,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>130</v>
       </c>
@@ -3681,7 +3680,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="38" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>133</v>
       </c>
@@ -3692,7 +3691,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>135</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -3725,7 +3724,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>137</v>
       </c>
@@ -3736,7 +3735,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -3758,7 +3757,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -3769,7 +3768,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="38" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
         <v>141</v>
       </c>
@@ -3780,7 +3779,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>142</v>
       </c>
@@ -3802,7 +3801,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>144</v>
       </c>
@@ -3813,7 +3812,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="32" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>145</v>
       </c>
@@ -3824,7 +3823,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="32" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>146</v>
       </c>
@@ -3835,7 +3834,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>147</v>
       </c>
@@ -3846,7 +3845,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="34" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
         <v>148</v>
       </c>
@@ -3857,7 +3856,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>149</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>151</v>
       </c>
@@ -3890,7 +3889,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>152</v>
       </c>
@@ -3901,7 +3900,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="32" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>154</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -3945,7 +3944,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>157</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -3968,11 +3967,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C43" xr:uid="{FB908553-6618-4CAE-8A24-8792C31B8736}">
-    <filterColumn colId="2">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C43" xr:uid="{FB908553-6618-4CAE-8A24-8792C31B8736}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
Backlog and Sprint updated
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Stevens\SSW555\Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F2C564-EAB1-4190-ABC5-45E07C3FAADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CE0AB6-A66D-43FD-B195-5A71545B29B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="206">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -690,6 +690,9 @@
   </si>
   <si>
     <t>Planned</t>
+  </si>
+  <si>
+    <t>Date before current dates</t>
   </si>
 </sst>
 </file>
@@ -1007,16 +1010,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BBB59"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2110,20 +2104,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="14" customWidth="1"/>
-    <col min="4" max="5" width="20.5" style="14" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="14" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" style="14" customWidth="1"/>
     <col min="6" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -2140,7 +2134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>197</v>
       </c>
@@ -2157,7 +2151,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>198</v>
       </c>
@@ -2174,7 +2168,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>199</v>
       </c>
@@ -2191,7 +2185,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>200</v>
       </c>
@@ -2208,7 +2202,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="13" t="s">
         <v>34</v>
       </c>
@@ -2237,19 +2231,19 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
@@ -2266,7 +2260,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -2283,7 +2277,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -2300,7 +2294,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="32" t="s">
         <v>144</v>
       </c>
@@ -2314,7 +2308,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
         <v>147</v>
       </c>
@@ -2328,7 +2322,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
         <v>149</v>
       </c>
@@ -2342,7 +2336,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
         <v>151</v>
       </c>
@@ -2356,7 +2350,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
         <v>152</v>
       </c>
@@ -2370,7 +2364,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="32" t="s">
         <v>154</v>
       </c>
@@ -2384,7 +2378,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>1</v>
+      </c>
       <c r="B10" s="38" t="s">
         <v>117</v>
       </c>
@@ -2395,10 +2392,13 @@
         <v>198</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>1</v>
+      </c>
       <c r="B11" s="38" t="s">
         <v>118</v>
       </c>
@@ -2409,10 +2409,10 @@
         <v>198</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
         <v>119</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="38" t="s">
         <v>122</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
         <v>123</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
         <v>133</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="38" t="s">
         <v>137</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>141</v>
       </c>
@@ -2496,7 +2496,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>1</v>
+      </c>
       <c r="B18" s="36" t="s">
         <v>120</v>
       </c>
@@ -2507,10 +2510,13 @@
         <v>200</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>1</v>
+      </c>
       <c r="B19" s="36" t="s">
         <v>121</v>
       </c>
@@ -2521,10 +2527,10 @@
         <v>200</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="36" t="s">
         <v>131</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="36" t="s">
         <v>132</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="36" t="s">
         <v>139</v>
       </c>
@@ -2566,7 +2572,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="36" t="s">
         <v>143</v>
       </c>
@@ -2580,7 +2586,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="36" t="s">
         <v>150</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="36" t="s">
         <v>156</v>
       </c>
@@ -2628,14 +2634,14 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="6"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="6"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2822,16 +2828,16 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2851,7 +2857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>42633</v>
       </c>
@@ -2865,7 +2871,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>42657</v>
       </c>
@@ -2875,7 +2881,7 @@
       <c r="E3" s="14"/>
       <c r="F3" s="20"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>42683</v>
       </c>
@@ -2885,7 +2891,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="20"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>42708</v>
       </c>
@@ -2895,7 +2901,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="20"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>42728</v>
       </c>
@@ -2917,25 +2923,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="16" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="14" customWidth="1"/>
     <col min="4" max="4" width="11" style="14"/>
-    <col min="5" max="5" width="6.875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="14" customWidth="1"/>
-    <col min="7" max="7" width="6.625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
@@ -2964,7 +2970,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>145</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>146</v>
       </c>
@@ -3022,13 +3028,25 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>205</v>
+      </c>
       <c r="C4" s="14" t="s">
         <v>198</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>194</v>
       </c>
+      <c r="E4" s="14">
+        <v>100</v>
+      </c>
+      <c r="F4" s="14">
+        <v>120</v>
+      </c>
       <c r="G4" s="14" t="s">
         <v>193</v>
       </c>
@@ -3039,13 +3057,25 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="C5" s="14" t="s">
         <v>198</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>194</v>
       </c>
+      <c r="E5" s="14">
+        <v>100</v>
+      </c>
+      <c r="F5" s="14">
+        <v>120</v>
+      </c>
       <c r="G5" s="14" t="s">
         <v>193</v>
       </c>
@@ -3056,7 +3086,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="14" t="s">
         <v>199</v>
       </c>
@@ -3073,7 +3103,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="14" t="s">
         <v>199</v>
       </c>
@@ -3090,13 +3120,25 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="C8" s="14" t="s">
         <v>200</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>194</v>
       </c>
+      <c r="E8" s="14">
+        <v>90</v>
+      </c>
+      <c r="F8" s="14">
+        <v>120</v>
+      </c>
       <c r="G8" s="14" t="s">
         <v>193</v>
       </c>
@@ -3107,13 +3149,25 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="C9" s="14" t="s">
         <v>200</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>194</v>
       </c>
+      <c r="E9" s="14">
+        <v>90</v>
+      </c>
+      <c r="F9" s="14">
+        <v>120</v>
+      </c>
       <c r="G9" s="14" t="s">
         <v>193</v>
       </c>
@@ -3124,35 +3178,35 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="16" t="s">
         <v>36</v>
       </c>
@@ -3172,9 +3226,9 @@
       <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
@@ -3203,7 +3257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -3214,7 +3268,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -3225,7 +3279,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -3236,7 +3290,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -3247,7 +3301,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -3258,7 +3312,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -3269,7 +3323,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -3280,7 +3334,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -3306,9 +3360,9 @@
       <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -3337,7 +3391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -3348,7 +3402,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -3359,7 +3413,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -3370,7 +3424,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -3381,7 +3435,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -3392,7 +3446,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -3403,7 +3457,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -3414,7 +3468,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -3439,12 +3493,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="11" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -3483,14 +3537,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3504,7 +3558,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="38" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>117</v>
       </c>
@@ -3515,7 +3569,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="38" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>118</v>
       </c>
@@ -3526,7 +3580,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="38" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>119</v>
       </c>
@@ -3537,7 +3591,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>120</v>
       </c>
@@ -3548,7 +3602,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>121</v>
       </c>
@@ -3559,7 +3613,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="38" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>122</v>
       </c>
@@ -3570,7 +3624,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="38" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="38" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>123</v>
       </c>
@@ -3581,7 +3635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -3592,7 +3646,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -3603,7 +3657,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -3614,7 +3668,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -3625,7 +3679,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -3636,7 +3690,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -3647,7 +3701,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>130</v>
       </c>
@@ -3658,7 +3712,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>131</v>
       </c>
@@ -3669,7 +3723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>132</v>
       </c>
@@ -3680,7 +3734,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="38" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>133</v>
       </c>
@@ -3691,7 +3745,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -3702,7 +3756,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>135</v>
       </c>
@@ -3713,7 +3767,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>136</v>
       </c>
@@ -3724,7 +3778,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="38" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>137</v>
       </c>
@@ -3735,7 +3789,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -3746,7 +3800,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>139</v>
       </c>
@@ -3757,7 +3811,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -3768,7 +3822,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="38" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="38" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
         <v>141</v>
       </c>
@@ -3779,7 +3833,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>142</v>
       </c>
@@ -3790,7 +3844,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
         <v>143</v>
       </c>
@@ -3801,7 +3855,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>144</v>
       </c>
@@ -3812,7 +3866,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>145</v>
       </c>
@@ -3823,7 +3877,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>146</v>
       </c>
@@ -3834,7 +3888,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>147</v>
       </c>
@@ -3845,7 +3899,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
         <v>148</v>
       </c>
@@ -3856,7 +3910,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>149</v>
       </c>
@@ -3867,7 +3921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="36" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>150</v>
       </c>
@@ -3878,7 +3932,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>151</v>
       </c>
@@ -3889,7 +3943,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>152</v>
       </c>
@@ -3900,7 +3954,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>153</v>
       </c>
@@ -3911,7 +3965,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>154</v>
       </c>
@@ -3922,7 +3976,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -3933,7 +3987,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>156</v>
       </c>
@@ -3944,7 +3998,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>157</v>
       </c>
@@ -3955,7 +4009,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
Stories added by Pradeep
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A7E093-E87A-4F88-9DFE-663E1BF9415B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -27,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$E$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$C$43</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="236">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -741,17 +735,59 @@
   </si>
   <si>
     <t>Sibiling spacing</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Pradeep</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>psentham@stevens.edu</t>
+  </si>
+  <si>
+    <t>Pradeep6149</t>
+  </si>
+  <si>
+    <t>US46</t>
+  </si>
+  <si>
+    <t>US47</t>
+  </si>
+  <si>
+    <t>US48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List living married Male </t>
+  </si>
+  <si>
+    <t>List living married Female</t>
+  </si>
+  <si>
+    <t>List all living married people who are male in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List all living married people who are female in a GEDCOM file</t>
+  </si>
+  <si>
+    <t>List people with single parent</t>
+  </si>
+  <si>
+    <t>List all people in a GEDCOM file who have either their father or their mother died in last 30 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -804,8 +840,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -845,6 +886,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,7 +1024,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -985,9 +1038,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1041,12 +1091,24 @@
     <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="65" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1135,7 +1197,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1206,7 +1268,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B4BC-4DF7-BB23-B148409AC56E}"/>
             </c:ext>
@@ -1222,11 +1284,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="50511232"/>
-        <c:axId val="62982400"/>
+        <c:axId val="205394304"/>
+        <c:axId val="205395840"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="50511232"/>
+        <c:axId val="205394304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1236,14 +1298,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62982400"/>
+        <c:crossAx val="205395840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62982400"/>
+        <c:axId val="205395840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1316,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50511232"/>
+        <c:crossAx val="205394304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,7 +1334,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1331,7 +1393,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C9EC-4DFB-9A9C-08D916B18EAB}"/>
             </c:ext>
@@ -1347,11 +1409,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66428928"/>
-        <c:axId val="66431616"/>
+        <c:axId val="204637696"/>
+        <c:axId val="204639232"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="66428928"/>
+        <c:axId val="204637696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1361,14 +1423,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66431616"/>
+        <c:crossAx val="204639232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="66431616"/>
+        <c:axId val="204639232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66428928"/>
+        <c:crossAx val="204637696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1416,7 +1478,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1454,7 +1516,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1529,7 +1591,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1594,7 +1656,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1663,7 +1725,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1733,7 +1795,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1802,7 +1864,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1872,7 +1934,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2212,137 +2274,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.90625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="14" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="14"/>
+    <col min="1" max="1" width="7.90625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="13" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="39" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="52"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <mergeCells count="1">
@@ -2350,644 +2429,766 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{D21ED74A-CE71-45F6-8383-B8F9C5E1D34F}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{014A5583-FAD3-4B3D-8AB2-19C06215DCA5}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.6328125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="14"/>
+    <col min="1" max="2" width="6.6328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>1</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>1</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <v>1</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="A19" s="13">
         <v>1</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
+      <c r="A28" s="13">
         <v>1</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
+      <c r="A32" s="13">
         <v>1</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+      <c r="A36" s="13">
         <v>1</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="39" t="s">
         <v>212</v>
       </c>
-      <c r="C39" s="40" t="s">
+      <c r="C39" s="39" t="s">
         <v>215</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="13" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+      <c r="A40" s="13">
         <v>1</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="13" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="39" t="s">
         <v>214</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="39" t="s">
         <v>219</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="13" t="s">
         <v>203</v>
       </c>
     </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
+        <v>1</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
+        <v>1</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>230</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="C48" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="53"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E25" xr:uid="{CF9EA074-D5DE-4C85-83F4-BAF6F52AE4EF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
+  <autoFilter ref="A1:E25">
+    <sortState ref="A2:E25">
       <sortCondition ref="A1:A25"/>
     </sortState>
   </autoFilter>
@@ -2998,7 +3199,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -3072,36 +3273,36 @@
       <c r="A15" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>41065</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>24</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>0</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>166</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>41078</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>250</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>120</v>
       </c>
       <c r="G16" s="8">
@@ -3113,20 +3314,20 @@
       <c r="A17" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>41092</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>12</v>
       </c>
       <c r="D17">
         <f>C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>480</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>135</v>
       </c>
       <c r="G17" s="8">
@@ -3138,20 +3339,20 @@
       <c r="A18" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>41106</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>6</v>
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D19" si="1">C17-C18</f>
         <v>6</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>740</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="11">
         <v>160</v>
       </c>
       <c r="G18" s="8">
@@ -3163,20 +3364,20 @@
       <c r="A19" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>41120</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>0</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>1100</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="11">
         <v>145</v>
       </c>
       <c r="G19" s="8">
@@ -3192,11 +3393,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3209,78 +3410,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+      <c r="A2" s="17">
         <v>42633</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>36</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13">
         <v>0</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="19"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="17">
         <v>42657</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="A4" s="17">
         <v>42683</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="17">
         <v>42708</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="17">
         <v>42728</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="19"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3291,376 +3492,434 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="11" style="14"/>
-    <col min="5" max="5" width="6.90625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="6.6328125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11" style="14"/>
+    <col min="1" max="1" width="7.6328125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="11" style="13"/>
+    <col min="5" max="5" width="6.90625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="7.453125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="7.6328125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>50</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <v>30</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>50</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>30</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>100</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>120</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>100</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>120</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>100</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>120</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>100</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>120</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>43</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>90</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="17">
         <v>42639</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>90</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>120</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>90</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>120</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>27</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>90</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="17">
         <v>42639</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>90</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>120</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>100</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>120</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="17" t="s">
         <v>193</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="13">
+        <v>100</v>
+      </c>
+      <c r="F12" s="13">
+        <v>120</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="13">
+        <v>90</v>
+      </c>
+      <c r="F13" s="13">
+        <v>120</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
+      <c r="B15" s="19"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3672,7 +3931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -3682,121 +3941,121 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3806,7 +4065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -3816,121 +4075,121 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3939,7 +4198,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -3948,35 +4207,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11" style="14"/>
+    <col min="1" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3987,11 +4246,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4011,503 +4270,536 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+    <row r="6" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:3" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+    <row r="9" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="37" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+    <row r="12" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="43" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+    <row r="13" spans="1:3" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="43" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="43" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+    <row r="14" spans="1:3" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="43" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+    <row r="15" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+    <row r="16" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+    <row r="17" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
+    <row r="18" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="43" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
+    <row r="20" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="35" t="s">
+    <row r="22" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="35" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="37" t="s">
+    <row r="23" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="33" t="s">
+    <row r="24" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="45" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="35" t="s">
+    <row r="26" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" s="44" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+      <c r="A27" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="45" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
+    <row r="28" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="31" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
+    <row r="31" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+    <row r="32" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="31" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="37" t="s">
+    <row r="33" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="37" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="31" t="s">
+    <row r="34" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="33" t="s">
+    <row r="35" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+    <row r="36" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
+    <row r="37" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A38" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="31" t="s">
+    <row r="39" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A39" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" s="37" t="s">
+    <row r="40" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="37" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" s="33" t="s">
+    <row r="41" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="45" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="37" t="s">
+    <row r="43" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="37" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="43" t="s">
+    <row r="44" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="43" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="43" t="s">
+    <row r="45" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A45" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="43" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="43" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A46" s="43" t="s">
+    <row r="46" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A46" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="C46" s="44" t="s">
+      <c r="C46" s="43" t="s">
         <v>220</v>
       </c>
     </row>
+    <row r="47" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="B47" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="A48" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="B48" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="A49" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C43" xr:uid="{FB908553-6618-4CAE-8A24-8792C31B8736}"/>
+  <autoFilter ref="A1:C43"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
Added US04 and test case
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A89CCF-4D4E-4F0E-A3D2-2F5D9AD5BE9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$E$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$C$43</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,6 +35,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -39,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="236">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -782,7 +789,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1102,13 +1109,13 @@
     <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="65" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1197,7 +1204,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1268,7 +1275,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B4BC-4DF7-BB23-B148409AC56E}"/>
             </c:ext>
@@ -1334,7 +1341,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1393,7 +1400,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C9EC-4DFB-9A9C-08D916B18EAB}"/>
             </c:ext>
@@ -1478,7 +1485,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1516,7 +1523,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1591,7 +1598,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,7 +1663,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1725,7 +1732,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1795,7 +1802,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1864,7 +1871,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1934,7 +1941,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2274,7 +2281,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -2414,14 +2421,14 @@
       <c r="D9" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="53"/>
     </row>
   </sheetData>
-  <sortState ref="A3:D5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <mergeCells count="1">
@@ -2429,12 +2436,12 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId7"/>
@@ -2442,11 +2449,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2725,7 +2732,7 @@
         <v>200</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2871,7 +2878,7 @@
         <v>199</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2930,7 +2937,7 @@
         <v>199</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3184,11 +3191,11 @@
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="53"/>
+      <c r="B50" s="51"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E25">
-    <sortState ref="A2:E25">
+  <autoFilter ref="A1:E25" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
       <sortCondition ref="A1:A25"/>
     </sortState>
   </autoFilter>
@@ -3199,7 +3206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -3393,7 +3400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -3492,11 +3499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3677,14 +3684,14 @@
       <c r="F6" s="13">
         <v>120</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>193</v>
+      <c r="G6" s="13">
+        <v>28</v>
+      </c>
+      <c r="H6" s="13">
+        <v>30</v>
+      </c>
+      <c r="I6" s="17">
+        <v>42644</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3735,14 +3742,14 @@
       <c r="F8" s="13">
         <v>120</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>193</v>
+      <c r="G8" s="13">
+        <v>21</v>
+      </c>
+      <c r="H8" s="13">
+        <v>90</v>
+      </c>
+      <c r="I8" s="17">
+        <v>42644</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3931,7 +3938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -4065,7 +4072,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -4198,7 +4205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -4246,11 +4253,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4799,7 +4806,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C43"/>
+  <autoFilter ref="A1:C43" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Sprint1 story and paired programming estimated time and lines of code.
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A89CCF-4D4E-4F0E-A3D2-2F5D9AD5BE9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4753A2E3-1D74-41E4-9C75-13CDC1E8B8FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="237">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -784,6 +783,9 @@
   </si>
   <si>
     <t>List all people in a GEDCOM file who have either their father or their mother died in last 30 days</t>
+  </si>
+  <si>
+    <t>List living Single (Paired Programming)</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1396,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2288,16 +2290,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.90625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="13" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="13" customWidth="1"/>
+    <col min="4" max="5" width="20.5" style="13" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -2314,7 +2316,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>197</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>198</v>
       </c>
@@ -2348,7 +2350,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>199</v>
       </c>
@@ -2365,7 +2367,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>200</v>
       </c>
@@ -2382,7 +2384,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>207</v>
       </c>
@@ -2399,7 +2401,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>222</v>
       </c>
@@ -2416,8 +2418,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D9" s="41" t="s">
         <v>34</v>
       </c>
@@ -2453,19 +2455,19 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B5" sqref="B5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.6328125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
@@ -2482,7 +2484,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2496,10 +2498,10 @@
         <v>197</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -2513,10 +2515,10 @@
         <v>197</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="22" t="s">
         <v>144</v>
       </c>
@@ -2530,7 +2532,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
       <c r="B5" s="22" t="s">
         <v>147</v>
       </c>
@@ -2541,10 +2546,10 @@
         <v>197</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="22" t="s">
         <v>149</v>
       </c>
@@ -2558,7 +2563,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="22" t="s">
         <v>151</v>
       </c>
@@ -2572,7 +2577,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="22" t="s">
         <v>152</v>
       </c>
@@ -2586,7 +2591,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
         <v>154</v>
       </c>
@@ -2600,7 +2605,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -2617,7 +2622,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>1</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="24" t="s">
         <v>119</v>
       </c>
@@ -2648,7 +2653,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="24" t="s">
         <v>122</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="24" t="s">
         <v>123</v>
       </c>
@@ -2676,7 +2681,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="24" t="s">
         <v>133</v>
       </c>
@@ -2690,7 +2695,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="24" t="s">
         <v>137</v>
       </c>
@@ -2704,7 +2709,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="24" t="s">
         <v>141</v>
       </c>
@@ -2718,7 +2723,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>1</v>
       </c>
@@ -2735,7 +2740,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -2752,7 +2757,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="28" t="s">
         <v>131</v>
       </c>
@@ -2766,7 +2771,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="28" t="s">
         <v>132</v>
       </c>
@@ -2780,7 +2785,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
         <v>139</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
         <v>143</v>
       </c>
@@ -2808,7 +2813,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="28" t="s">
         <v>150</v>
       </c>
@@ -2822,7 +2827,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="28" t="s">
         <v>156</v>
       </c>
@@ -2836,7 +2841,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="s">
         <v>124</v>
       </c>
@@ -2850,7 +2855,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="s">
         <v>125</v>
       </c>
@@ -2864,7 +2869,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>1</v>
       </c>
@@ -2881,7 +2886,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
         <v>130</v>
       </c>
@@ -2895,7 +2900,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="26" t="s">
         <v>138</v>
       </c>
@@ -2909,7 +2914,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" s="26" t="s">
         <v>148</v>
       </c>
@@ -2923,7 +2928,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>1</v>
       </c>
@@ -2940,7 +2945,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
         <v>158</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" s="39" t="s">
         <v>127</v>
       </c>
@@ -2968,7 +2973,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="39" t="s">
         <v>128</v>
       </c>
@@ -2982,7 +2987,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>1</v>
       </c>
@@ -2999,7 +3004,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" s="39" t="s">
         <v>134</v>
       </c>
@@ -3013,7 +3018,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="39" t="s">
         <v>135</v>
       </c>
@@ -3027,7 +3032,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="39" t="s">
         <v>212</v>
       </c>
@@ -3041,7 +3046,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>1</v>
       </c>
@@ -3058,7 +3063,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="39" t="s">
         <v>214</v>
       </c>
@@ -3072,7 +3077,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <v>1</v>
       </c>
@@ -3089,7 +3094,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="47" t="s">
         <v>140</v>
       </c>
@@ -3103,7 +3108,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="47" t="s">
         <v>142</v>
       </c>
@@ -3117,7 +3122,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" s="47" t="s">
         <v>153</v>
       </c>
@@ -3131,7 +3136,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <v>1</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47" s="47" t="s">
         <v>227</v>
       </c>
@@ -3162,7 +3167,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="47" t="s">
         <v>228</v>
       </c>
@@ -3176,7 +3181,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="47" t="s">
         <v>229</v>
       </c>
@@ -3190,7 +3195,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="51"/>
     </row>
   </sheetData>
@@ -3213,14 +3218,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="6"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="6"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3404,19 +3409,19 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3436,12 +3441,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>42633</v>
       </c>
       <c r="B2" s="13">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13">
@@ -3450,7 +3455,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>42657</v>
       </c>
@@ -3460,7 +3465,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>42683</v>
       </c>
@@ -3470,7 +3475,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>42708</v>
       </c>
@@ -3480,7 +3485,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>42728</v>
       </c>
@@ -3500,27 +3505,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="13" customWidth="1"/>
     <col min="4" max="4" width="11" style="13"/>
-    <col min="5" max="5" width="6.90625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="6.6328125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="13" customWidth="1"/>
+    <col min="7" max="7" width="6.625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -3549,7 +3554,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -3560,25 +3565,25 @@
         <v>197</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E2" s="13">
         <v>50</v>
       </c>
       <c r="F2" s="13">
-        <v>30</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="G2" s="13">
+        <v>33</v>
+      </c>
+      <c r="H2" s="13">
+        <v>90</v>
+      </c>
+      <c r="I2" s="17">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>146</v>
       </c>
@@ -3589,59 +3594,59 @@
         <v>197</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E3" s="13">
         <v>50</v>
       </c>
       <c r="F3" s="13">
-        <v>30</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="G3" s="13">
+        <v>11</v>
+      </c>
+      <c r="H3" s="13">
+        <v>60</v>
+      </c>
+      <c r="I3" s="17">
+        <v>42646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>205</v>
+        <v>147</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>236</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E4" s="13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F4" s="13">
         <v>120</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="13">
+        <v>12</v>
+      </c>
+      <c r="H4" s="13">
+        <v>50</v>
+      </c>
+      <c r="I4" s="17">
+        <v>42646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>72</v>
+        <v>205</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>198</v>
@@ -3665,15 +3670,15 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>80</v>
+        <v>118</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>194</v>
@@ -3684,22 +3689,22 @@
       <c r="F6" s="13">
         <v>120</v>
       </c>
-      <c r="G6" s="13">
-        <v>28</v>
-      </c>
-      <c r="H6" s="13">
-        <v>30</v>
-      </c>
-      <c r="I6" s="17">
-        <v>42644</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>199</v>
@@ -3714,50 +3719,50 @@
         <v>120</v>
       </c>
       <c r="G7" s="13">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H7" s="13">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="I7" s="17">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>73</v>
+        <v>155</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>110</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>194</v>
       </c>
       <c r="E8" s="13">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F8" s="13">
         <v>120</v>
       </c>
       <c r="G8" s="13">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="H8" s="13">
         <v>90</v>
       </c>
       <c r="I8" s="17">
-        <v>42644</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>200</v>
@@ -3772,24 +3777,24 @@
         <v>120</v>
       </c>
       <c r="G9" s="13">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H9" s="13">
         <v>90</v>
       </c>
       <c r="I9" s="17">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42644</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>213</v>
+        <v>121</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>221</v>
+        <v>74</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>194</v>
@@ -3800,22 +3805,22 @@
       <c r="F10" s="13">
         <v>120</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="13">
+        <v>27</v>
+      </c>
+      <c r="H10" s="13">
+        <v>90</v>
+      </c>
+      <c r="I10" s="17">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>129</v>
+        <v>213</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>207</v>
@@ -3824,7 +3829,7 @@
         <v>194</v>
       </c>
       <c r="E11" s="13">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F11" s="13">
         <v>120</v>
@@ -3839,15 +3844,15 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>194</v>
@@ -3868,12 +3873,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>222</v>
@@ -3882,7 +3887,7 @@
         <v>194</v>
       </c>
       <c r="E13" s="13">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F13" s="13">
         <v>120</v>
@@ -3897,36 +3902,65 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="13">
+        <v>90</v>
+      </c>
+      <c r="F14" s="13">
+        <v>120</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="19"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+    <row r="22" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3945,9 +3979,9 @@
       <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -3976,7 +4010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -3987,7 +4021,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -3998,7 +4032,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4009,7 +4043,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4020,7 +4054,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4031,7 +4065,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4042,7 +4076,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4053,7 +4087,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4079,9 +4113,9 @@
       <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4110,7 +4144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -4121,7 +4155,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -4132,7 +4166,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4143,7 +4177,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4154,7 +4188,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4165,7 +4199,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4176,7 +4210,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4187,7 +4221,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4212,12 +4246,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4256,14 +4290,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4277,7 +4311,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>117</v>
       </c>
@@ -4288,7 +4322,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>118</v>
       </c>
@@ -4299,7 +4333,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>119</v>
       </c>
@@ -4310,7 +4344,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>120</v>
       </c>
@@ -4321,7 +4355,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>121</v>
       </c>
@@ -4332,7 +4366,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>122</v>
       </c>
@@ -4343,7 +4377,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="34" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>123</v>
       </c>
@@ -4354,7 +4388,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>124</v>
       </c>
@@ -4365,7 +4399,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>125</v>
       </c>
@@ -4376,7 +4410,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>126</v>
       </c>
@@ -4387,7 +4421,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
         <v>127</v>
       </c>
@@ -4398,7 +4432,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="42" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
         <v>128</v>
       </c>
@@ -4409,7 +4443,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="42" customFormat="1" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
         <v>129</v>
       </c>
@@ -4420,7 +4454,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>130</v>
       </c>
@@ -4431,7 +4465,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>131</v>
       </c>
@@ -4442,7 +4476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
@@ -4453,7 +4487,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
         <v>133</v>
       </c>
@@ -4464,7 +4498,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="42" t="s">
         <v>134</v>
       </c>
@@ -4475,7 +4509,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="42" t="s">
         <v>135</v>
       </c>
@@ -4486,7 +4520,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
         <v>136</v>
       </c>
@@ -4497,7 +4531,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>137</v>
       </c>
@@ -4508,7 +4542,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>138</v>
       </c>
@@ -4519,7 +4553,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>139</v>
       </c>
@@ -4530,7 +4564,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="44" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" s="44" t="s">
         <v>140</v>
       </c>
@@ -4541,7 +4575,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" s="34" t="s">
         <v>141</v>
       </c>
@@ -4552,7 +4586,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="44" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" s="44" t="s">
         <v>142</v>
       </c>
@@ -4563,7 +4597,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>143</v>
       </c>
@@ -4574,7 +4608,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>144</v>
       </c>
@@ -4585,7 +4619,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>145</v>
       </c>
@@ -4596,7 +4630,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
         <v>146</v>
       </c>
@@ -4607,7 +4641,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>147</v>
       </c>
@@ -4618,7 +4652,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
         <v>148</v>
       </c>
@@ -4629,7 +4663,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>149</v>
       </c>
@@ -4640,7 +4674,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="32" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>150</v>
       </c>
@@ -4651,7 +4685,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
         <v>151</v>
       </c>
@@ -4662,7 +4696,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
         <v>152</v>
       </c>
@@ -4673,7 +4707,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
         <v>153</v>
       </c>
@@ -4684,7 +4718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>154</v>
       </c>
@@ -4695,7 +4729,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>155</v>
       </c>
@@ -4706,7 +4740,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>156</v>
       </c>
@@ -4717,7 +4751,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
         <v>157</v>
       </c>
@@ -4728,7 +4762,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>158</v>
       </c>
@@ -4739,7 +4773,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="42" t="s">
         <v>212</v>
       </c>
@@ -4750,7 +4784,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
         <v>213</v>
       </c>
@@ -4761,7 +4795,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
         <v>214</v>
       </c>
@@ -4772,7 +4806,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="46" t="s">
         <v>227</v>
       </c>
@@ -4783,7 +4817,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="46" t="s">
         <v>228</v>
       </c>
@@ -4794,7 +4828,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="46" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Updated paired programming assignee for user story 31
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4753A2E3-1D74-41E4-9C75-13CDC1E8B8FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9557266-6038-44EE-9268-4AA94E1A60DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="238">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -786,6 +786,9 @@
   </si>
   <si>
     <t>List living Single (Paired Programming)</t>
+  </si>
+  <si>
+    <t>DA/AA</t>
   </si>
 </sst>
 </file>
@@ -3508,7 +3511,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3620,7 +3623,7 @@
         <v>236</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>206</v>
@@ -3959,7 +3962,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Updating the files with the Sprint details
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/CS561/CS_555_Project-hw05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9557266-6038-44EE-9268-4AA94E1A60DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90AD626-CB8D-5B4A-82C0-FE661B339955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="240">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -789,6 +789,12 @@
   </si>
   <si>
     <t>DA/AA</t>
+  </si>
+  <si>
+    <t>Birth before marriage(Paired Programming)</t>
+  </si>
+  <si>
+    <t>AA/DA</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1241,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1306,7 +1312,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2293,16 +2299,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="13" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="13" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="22" t="s">
         <v>197</v>
       </c>
@@ -2336,7 +2342,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
         <v>198</v>
       </c>
@@ -2353,7 +2359,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>199</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
         <v>200</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="39" t="s">
         <v>207</v>
       </c>
@@ -2404,7 +2410,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="47" t="s">
         <v>222</v>
       </c>
@@ -2421,8 +2427,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D9" s="41" t="s">
         <v>34</v>
       </c>
@@ -2458,19 +2464,19 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="6.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
@@ -2487,7 +2493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -2521,7 +2527,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="22" t="s">
         <v>144</v>
       </c>
@@ -2535,7 +2541,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" s="22" t="s">
         <v>149</v>
       </c>
@@ -2566,7 +2572,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" s="22" t="s">
         <v>151</v>
       </c>
@@ -2580,7 +2586,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B8" s="22" t="s">
         <v>152</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" s="22" t="s">
         <v>154</v>
       </c>
@@ -2608,7 +2614,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -2622,10 +2628,10 @@
         <v>198</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>1</v>
       </c>
@@ -2639,10 +2645,10 @@
         <v>198</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" s="24" t="s">
         <v>119</v>
       </c>
@@ -2656,7 +2662,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" s="24" t="s">
         <v>122</v>
       </c>
@@ -2670,7 +2676,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" s="24" t="s">
         <v>123</v>
       </c>
@@ -2684,7 +2690,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" s="24" t="s">
         <v>133</v>
       </c>
@@ -2698,7 +2704,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" s="24" t="s">
         <v>137</v>
       </c>
@@ -2712,7 +2718,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" s="24" t="s">
         <v>141</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>1</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -2760,7 +2766,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" s="28" t="s">
         <v>131</v>
       </c>
@@ -2774,7 +2780,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" s="28" t="s">
         <v>132</v>
       </c>
@@ -2788,7 +2794,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" s="28" t="s">
         <v>139</v>
       </c>
@@ -2802,7 +2808,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B23" s="28" t="s">
         <v>143</v>
       </c>
@@ -2816,7 +2822,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B24" s="28" t="s">
         <v>150</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" s="28" t="s">
         <v>156</v>
       </c>
@@ -2844,7 +2850,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" s="26" t="s">
         <v>124</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B27" s="26" t="s">
         <v>125</v>
       </c>
@@ -2872,7 +2878,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>1</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B29" s="26" t="s">
         <v>130</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B30" s="26" t="s">
         <v>138</v>
       </c>
@@ -2917,7 +2923,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B31" s="26" t="s">
         <v>148</v>
       </c>
@@ -2931,7 +2937,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>1</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" s="26" t="s">
         <v>158</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" s="39" t="s">
         <v>127</v>
       </c>
@@ -2976,7 +2982,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" s="39" t="s">
         <v>128</v>
       </c>
@@ -2990,7 +2996,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="13">
         <v>1</v>
       </c>
@@ -3007,7 +3013,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B37" s="39" t="s">
         <v>134</v>
       </c>
@@ -3021,7 +3027,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B38" s="39" t="s">
         <v>135</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B39" s="39" t="s">
         <v>212</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="13">
         <v>1</v>
       </c>
@@ -3066,7 +3072,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" s="39" t="s">
         <v>214</v>
       </c>
@@ -3080,7 +3086,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="13">
         <v>1</v>
       </c>
@@ -3097,7 +3103,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" s="47" t="s">
         <v>140</v>
       </c>
@@ -3111,7 +3117,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B44" s="47" t="s">
         <v>142</v>
       </c>
@@ -3125,7 +3131,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B45" s="47" t="s">
         <v>153</v>
       </c>
@@ -3139,7 +3145,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="13">
         <v>1</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B47" s="47" t="s">
         <v>227</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B48" s="47" t="s">
         <v>228</v>
       </c>
@@ -3184,7 +3190,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B49" s="47" t="s">
         <v>229</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B50" s="51"/>
     </row>
   </sheetData>
@@ -3221,47 +3227,47 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="6"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>164</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -3300,7 +3306,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -3325,7 +3331,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>167</v>
       </c>
@@ -3350,7 +3356,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>168</v>
       </c>
@@ -3375,7 +3381,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>169</v>
       </c>
@@ -3415,16 +3421,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3444,7 +3450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="17">
         <v>42633</v>
       </c>
@@ -3458,7 +3464,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="17">
         <v>42657</v>
       </c>
@@ -3468,7 +3474,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>42683</v>
       </c>
@@ -3478,7 +3484,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="17">
         <v>42708</v>
       </c>
@@ -3488,7 +3494,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="17">
         <v>42728</v>
       </c>
@@ -3510,25 +3516,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="13" customWidth="1"/>
     <col min="4" max="4" width="11" style="13"/>
-    <col min="5" max="5" width="6.875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="13" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="13" customWidth="1"/>
-    <col min="7" max="7" width="6.625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -3557,7 +3563,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>146</v>
       </c>
@@ -3615,7 +3621,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
         <v>147</v>
       </c>
@@ -3644,7 +3650,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>117</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>198</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E5" s="13">
         <v>100</v>
@@ -3663,28 +3669,28 @@
       <c r="F5" s="13">
         <v>120</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5" s="13">
+        <v>15</v>
+      </c>
+      <c r="H5" s="13">
+        <v>60</v>
+      </c>
+      <c r="I5" s="17">
+        <v>42646</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>118</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>72</v>
+        <v>238</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>198</v>
+        <v>239</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E6" s="13">
         <v>100</v>
@@ -3692,17 +3698,17 @@
       <c r="F6" s="13">
         <v>120</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6" s="13">
+        <v>15</v>
+      </c>
+      <c r="H6" s="13">
+        <v>60</v>
+      </c>
+      <c r="I6" s="17">
+        <v>42646</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
         <v>126</v>
       </c>
@@ -3731,7 +3737,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
         <v>155</v>
       </c>
@@ -3760,7 +3766,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -3789,7 +3795,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -3818,7 +3824,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
         <v>213</v>
       </c>
@@ -3847,7 +3853,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
         <v>129</v>
       </c>
@@ -3876,7 +3882,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
         <v>157</v>
       </c>
@@ -3905,7 +3911,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="13" t="s">
         <v>136</v>
       </c>
@@ -3934,35 +3940,35 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B16" s="19"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="14" t="s">
         <v>36</v>
       </c>
@@ -3982,9 +3988,9 @@
       <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -4024,7 +4030,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -4035,7 +4041,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4046,7 +4052,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4057,7 +4063,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4068,7 +4074,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4079,7 +4085,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4090,7 +4096,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4116,9 +4122,9 @@
       <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4147,7 +4153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -4158,7 +4164,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -4169,7 +4175,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4180,7 +4186,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4191,7 +4197,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4202,7 +4208,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4213,7 +4219,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4224,7 +4230,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4249,12 +4255,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4293,17 +4299,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>116</v>
       </c>
@@ -4314,7 +4320,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
         <v>117</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
         <v>118</v>
       </c>
@@ -4336,7 +4342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="34" t="s">
         <v>119</v>
       </c>
@@ -4347,7 +4353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>120</v>
       </c>
@@ -4358,7 +4364,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>121</v>
       </c>
@@ -4369,7 +4375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="34" t="s">
         <v>122</v>
       </c>
@@ -4380,7 +4386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="34" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="34" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="34" t="s">
         <v>123</v>
       </c>
@@ -4391,7 +4397,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="36" t="s">
         <v>124</v>
       </c>
@@ -4402,7 +4408,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="36" t="s">
         <v>125</v>
       </c>
@@ -4413,7 +4419,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="36" t="s">
         <v>126</v>
       </c>
@@ -4424,7 +4430,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="42" t="s">
         <v>127</v>
       </c>
@@ -4435,7 +4441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="42" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="42" t="s">
         <v>128</v>
       </c>
@@ -4446,7 +4452,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="42" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" s="42" t="s">
         <v>129</v>
       </c>
@@ -4457,7 +4463,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="36" t="s">
         <v>130</v>
       </c>
@@ -4468,7 +4474,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>131</v>
       </c>
@@ -4479,7 +4485,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="34" t="s">
         <v>133</v>
       </c>
@@ -4501,7 +4507,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="42" t="s">
         <v>134</v>
       </c>
@@ -4512,7 +4518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="42" t="s">
         <v>135</v>
       </c>
@@ -4523,7 +4529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="44" t="s">
         <v>136</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="34" t="s">
         <v>137</v>
       </c>
@@ -4545,7 +4551,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" s="36" t="s">
         <v>138</v>
       </c>
@@ -4556,7 +4562,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
         <v>139</v>
       </c>
@@ -4567,7 +4573,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="44" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="44" t="s">
         <v>140</v>
       </c>
@@ -4578,7 +4584,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="34" t="s">
         <v>141</v>
       </c>
@@ -4589,7 +4595,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="44" customFormat="1" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" s="44" t="s">
         <v>142</v>
       </c>
@@ -4600,7 +4606,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" s="32" t="s">
         <v>143</v>
       </c>
@@ -4611,7 +4617,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="30" t="s">
         <v>144</v>
       </c>
@@ -4622,7 +4628,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="30" t="s">
         <v>145</v>
       </c>
@@ -4633,7 +4639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="30" t="s">
         <v>146</v>
       </c>
@@ -4644,7 +4650,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="30" t="s">
         <v>147</v>
       </c>
@@ -4655,7 +4661,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="36" t="s">
         <v>148</v>
       </c>
@@ -4666,7 +4672,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" s="30" t="s">
         <v>149</v>
       </c>
@@ -4677,7 +4683,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="32" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="32" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" s="32" t="s">
         <v>150</v>
       </c>
@@ -4688,7 +4694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="30" t="s">
         <v>151</v>
       </c>
@@ -4699,7 +4705,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" s="30" t="s">
         <v>152</v>
       </c>
@@ -4710,7 +4716,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" s="44" t="s">
         <v>153</v>
       </c>
@@ -4721,7 +4727,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" s="30" t="s">
         <v>154</v>
       </c>
@@ -4732,7 +4738,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" s="36" t="s">
         <v>155</v>
       </c>
@@ -4743,7 +4749,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" s="32" t="s">
         <v>156</v>
       </c>
@@ -4754,7 +4760,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" s="44" t="s">
         <v>157</v>
       </c>
@@ -4765,7 +4771,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" s="36" t="s">
         <v>158</v>
       </c>
@@ -4776,7 +4782,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A44" s="42" t="s">
         <v>212</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A45" s="42" t="s">
         <v>213</v>
       </c>
@@ -4798,7 +4804,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A46" s="42" t="s">
         <v>214</v>
       </c>
@@ -4809,7 +4815,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A47" s="46" t="s">
         <v>227</v>
       </c>
@@ -4820,7 +4826,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="46" t="s">
         <v>228</v>
       </c>
@@ -4831,7 +4837,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A49" s="46" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Corrected Actual time of paired programming under sprint1 tab
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anuragaman/Desktop/CS561/CS_555_Project-hw05/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90AD626-CB8D-5B4A-82C0-FE661B339955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E308DA92-50BC-4586-9266-1C9CE7E3C9D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1241,7 +1241,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1312,7 +1312,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2299,16 +2299,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="13" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="13" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>197</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>198</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>199</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>200</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>207</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>222</v>
       </c>
@@ -2427,8 +2427,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D9" s="41" t="s">
         <v>34</v>
       </c>
@@ -2467,16 +2467,16 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="22" t="s">
         <v>144</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="22" t="s">
         <v>149</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="22" t="s">
         <v>151</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="22" t="s">
         <v>152</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
         <v>154</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>1</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="24" t="s">
         <v>119</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="24" t="s">
         <v>122</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="24" t="s">
         <v>123</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="24" t="s">
         <v>133</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="24" t="s">
         <v>137</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="24" t="s">
         <v>141</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>1</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="28" t="s">
         <v>131</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="28" t="s">
         <v>132</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
         <v>139</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
         <v>143</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="28" t="s">
         <v>150</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="28" t="s">
         <v>156</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="s">
         <v>124</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="s">
         <v>125</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>1</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
         <v>130</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="26" t="s">
         <v>138</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" s="26" t="s">
         <v>148</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>1</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
         <v>158</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" s="39" t="s">
         <v>127</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="39" t="s">
         <v>128</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>1</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" s="39" t="s">
         <v>134</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="39" t="s">
         <v>135</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="39" t="s">
         <v>212</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>1</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="39" t="s">
         <v>214</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <v>1</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="47" t="s">
         <v>140</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="47" t="s">
         <v>142</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" s="47" t="s">
         <v>153</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <v>1</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47" s="47" t="s">
         <v>227</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="47" t="s">
         <v>228</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="47" t="s">
         <v>229</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="51"/>
     </row>
   </sheetData>
@@ -3227,47 +3227,47 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="6"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>164</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -3306,7 +3306,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>167</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>168</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>169</v>
       </c>
@@ -3421,16 +3421,16 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>42633</v>
       </c>
@@ -3464,7 +3464,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>42657</v>
       </c>
@@ -3474,7 +3474,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>42683</v>
       </c>
@@ -3484,7 +3484,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>42708</v>
       </c>
@@ -3494,7 +3494,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>42728</v>
       </c>
@@ -3516,25 +3516,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="13" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="13" customWidth="1"/>
     <col min="4" max="4" width="11" style="13"/>
-    <col min="5" max="5" width="6.83203125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="13" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="13" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>146</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>147</v>
       </c>
@@ -3644,13 +3644,13 @@
         <v>12</v>
       </c>
       <c r="H4" s="13">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I4" s="17">
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>117</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>118</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>126</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>155</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>213</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>129</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>157</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>136</v>
       </c>
@@ -3940,35 +3940,35 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="19"/>
     </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
         <v>36</v>
       </c>
@@ -3988,9 +3988,9 @@
       <selection activeCell="C2" sqref="C2:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -4030,7 +4030,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -4041,7 +4041,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4052,7 +4052,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4063,7 +4063,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4074,7 +4074,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4085,7 +4085,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4096,7 +4096,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4122,9 +4122,9 @@
       <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -4164,7 +4164,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -4175,7 +4175,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4186,7 +4186,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4197,7 +4197,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4208,7 +4208,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4219,7 +4219,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4230,7 +4230,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4255,12 +4255,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4299,17 +4299,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>116</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>117</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>118</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>119</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>120</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>121</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>122</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="34" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" s="34" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>123</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>124</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>125</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>126</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
         <v>127</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" s="42" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
         <v>128</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" s="42" customFormat="1" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
         <v>129</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>130</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>131</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
         <v>133</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="42" t="s">
         <v>134</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="42" t="s">
         <v>135</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
         <v>136</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>137</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>138</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>139</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" s="44" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" s="44" t="s">
         <v>140</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" s="34" t="s">
         <v>141</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="44" customFormat="1" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" s="44" t="s">
         <v>142</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>143</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>144</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>145</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
         <v>146</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>147</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
         <v>148</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>149</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="32" customFormat="1" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" s="32" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>150</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
         <v>151</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
         <v>152</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
         <v>153</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>154</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>155</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>156</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
         <v>157</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>158</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="42" t="s">
         <v>212</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
         <v>213</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
         <v>214</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="46" t="s">
         <v>227</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="46" t="s">
         <v>228</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="46" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Updated Sprint 2 stories
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens Institute of Technology\3rd Sem\CS-555\Project\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CB1F04-F4FA-482C-A249-2EC0AB792A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA1DE3F-5DE9-4FC4-BF7F-0B3245274631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="242">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2306,16 +2305,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.90625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" style="13" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="13" customWidth="1"/>
+    <col min="4" max="5" width="20.5" style="13" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>197</v>
       </c>
@@ -2349,7 +2348,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>198</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>199</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>200</v>
       </c>
@@ -2400,7 +2399,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
         <v>207</v>
       </c>
@@ -2417,7 +2416,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>222</v>
       </c>
@@ -2434,8 +2433,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D9" s="41" t="s">
         <v>34</v>
       </c>
@@ -2470,20 +2469,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.6328125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
@@ -2500,7 +2499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2517,7 +2516,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="22" t="s">
         <v>144</v>
       </c>
@@ -2548,7 +2547,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -2565,7 +2564,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="22" t="s">
         <v>149</v>
       </c>
@@ -2579,7 +2578,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>2</v>
+      </c>
       <c r="B7" s="22" t="s">
         <v>151</v>
       </c>
@@ -2590,10 +2592,13 @@
         <v>197</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>2</v>
+      </c>
       <c r="B8" s="22" t="s">
         <v>152</v>
       </c>
@@ -2604,10 +2609,10 @@
         <v>197</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
         <v>154</v>
       </c>
@@ -2621,7 +2626,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -2638,7 +2643,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>1</v>
       </c>
@@ -2655,7 +2660,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="24" t="s">
         <v>119</v>
       </c>
@@ -2669,7 +2674,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="24" t="s">
         <v>122</v>
       </c>
@@ -2683,7 +2688,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="24" t="s">
         <v>123</v>
       </c>
@@ -2697,7 +2702,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="24" t="s">
         <v>133</v>
       </c>
@@ -2711,7 +2716,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="24" t="s">
         <v>137</v>
       </c>
@@ -2725,7 +2730,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="24" t="s">
         <v>141</v>
       </c>
@@ -2739,7 +2744,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>1</v>
       </c>
@@ -2756,7 +2761,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -2773,7 +2778,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="28" t="s">
         <v>131</v>
       </c>
@@ -2787,7 +2792,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="28" t="s">
         <v>132</v>
       </c>
@@ -2801,7 +2806,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
         <v>139</v>
       </c>
@@ -2815,7 +2820,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
         <v>143</v>
       </c>
@@ -2829,7 +2834,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="28" t="s">
         <v>150</v>
       </c>
@@ -2843,7 +2848,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="28" t="s">
         <v>156</v>
       </c>
@@ -2857,7 +2862,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="s">
         <v>124</v>
       </c>
@@ -2871,7 +2876,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="s">
         <v>125</v>
       </c>
@@ -2885,7 +2890,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>1</v>
       </c>
@@ -2902,7 +2907,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
         <v>130</v>
       </c>
@@ -2916,7 +2921,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="26" t="s">
         <v>138</v>
       </c>
@@ -2930,7 +2935,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" s="26" t="s">
         <v>148</v>
       </c>
@@ -2944,7 +2949,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>1</v>
       </c>
@@ -2961,7 +2966,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
         <v>158</v>
       </c>
@@ -2975,7 +2980,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" s="39" t="s">
         <v>127</v>
       </c>
@@ -2989,7 +2994,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="39" t="s">
         <v>128</v>
       </c>
@@ -3003,7 +3008,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>1</v>
       </c>
@@ -3020,7 +3025,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" s="39" t="s">
         <v>134</v>
       </c>
@@ -3034,7 +3039,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="39" t="s">
         <v>135</v>
       </c>
@@ -3048,7 +3053,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="39" t="s">
         <v>212</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>1</v>
       </c>
@@ -3079,7 +3084,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="39" t="s">
         <v>214</v>
       </c>
@@ -3093,7 +3098,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B42" s="47" t="s">
         <v>136</v>
       </c>
@@ -3107,7 +3112,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="47" t="s">
         <v>140</v>
       </c>
@@ -3121,7 +3126,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="47" t="s">
         <v>142</v>
       </c>
@@ -3135,7 +3140,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" s="47" t="s">
         <v>153</v>
       </c>
@@ -3149,7 +3154,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46" s="47" t="s">
         <v>157</v>
       </c>
@@ -3163,7 +3168,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
         <v>1</v>
       </c>
@@ -3180,7 +3185,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="47" t="s">
         <v>228</v>
       </c>
@@ -3194,7 +3199,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="13">
         <v>1</v>
       </c>
@@ -3211,7 +3216,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" s="51"/>
     </row>
   </sheetData>
@@ -3234,14 +3239,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="6"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="6"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3428,16 +3433,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3457,7 +3462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>42633</v>
       </c>
@@ -3471,7 +3476,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>42657</v>
       </c>
@@ -3481,7 +3486,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>42683</v>
       </c>
@@ -3491,7 +3496,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>42708</v>
       </c>
@@ -3501,7 +3506,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>42728</v>
       </c>
@@ -3524,24 +3529,24 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="13" customWidth="1"/>
     <col min="4" max="4" width="11" style="13"/>
-    <col min="5" max="5" width="6.90625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="6.6328125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="13" customWidth="1"/>
+    <col min="7" max="7" width="6.625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -3570,7 +3575,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -3599,7 +3604,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>146</v>
       </c>
@@ -3628,7 +3633,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>147</v>
       </c>
@@ -3657,7 +3662,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>117</v>
       </c>
@@ -3686,7 +3691,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>118</v>
       </c>
@@ -3715,7 +3720,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>126</v>
       </c>
@@ -3744,7 +3749,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>155</v>
       </c>
@@ -3773,7 +3778,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -3802,7 +3807,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -3831,7 +3836,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>213</v>
       </c>
@@ -3860,7 +3865,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>129</v>
       </c>
@@ -3889,7 +3894,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>227</v>
       </c>
@@ -3918,7 +3923,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>229</v>
       </c>
@@ -3947,35 +3952,35 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="19"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="14" t="s">
         <v>36</v>
       </c>
@@ -3991,13 +3996,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -4026,29 +4031,53 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="13">
+        <v>25</v>
+      </c>
+      <c r="F2" s="13">
+        <v>60</v>
+      </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="13">
+        <v>25</v>
+      </c>
+      <c r="F3" s="13">
+        <v>60</v>
+      </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4059,7 +4088,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4070,7 +4099,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4081,7 +4110,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4092,7 +4121,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4103,7 +4132,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4129,9 +4158,9 @@
       <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4160,7 +4189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -4171,7 +4200,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -4182,7 +4211,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4193,7 +4222,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4204,7 +4233,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4215,7 +4244,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4226,7 +4255,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4237,7 +4266,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4262,12 +4291,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4306,14 +4335,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4327,7 +4356,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
         <v>117</v>
       </c>
@@ -4338,7 +4367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>118</v>
       </c>
@@ -4349,7 +4378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>119</v>
       </c>
@@ -4360,7 +4389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>120</v>
       </c>
@@ -4371,7 +4400,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>121</v>
       </c>
@@ -4382,7 +4411,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
         <v>122</v>
       </c>
@@ -4393,7 +4422,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="34" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" s="34" t="s">
         <v>123</v>
       </c>
@@ -4404,7 +4433,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>124</v>
       </c>
@@ -4415,7 +4444,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>125</v>
       </c>
@@ -4426,7 +4455,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>126</v>
       </c>
@@ -4437,7 +4466,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" s="42" t="s">
         <v>127</v>
       </c>
@@ -4448,7 +4477,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="42" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" s="42" t="s">
         <v>128</v>
       </c>
@@ -4459,7 +4488,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="42" customFormat="1" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" s="42" t="s">
         <v>129</v>
       </c>
@@ -4470,7 +4499,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>130</v>
       </c>
@@ -4481,7 +4510,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>131</v>
       </c>
@@ -4492,7 +4521,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
@@ -4503,7 +4532,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="34" t="s">
         <v>133</v>
       </c>
@@ -4514,7 +4543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="42" t="s">
         <v>134</v>
       </c>
@@ -4525,7 +4554,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="42" t="s">
         <v>135</v>
       </c>
@@ -4536,7 +4565,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" s="44" t="s">
         <v>136</v>
       </c>
@@ -4547,7 +4576,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
         <v>137</v>
       </c>
@@ -4558,7 +4587,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>138</v>
       </c>
@@ -4569,7 +4598,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>139</v>
       </c>
@@ -4580,7 +4609,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="44" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" s="44" t="s">
         <v>140</v>
       </c>
@@ -4591,7 +4620,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" s="34" t="s">
         <v>141</v>
       </c>
@@ -4602,7 +4631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="44" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" s="44" t="s">
         <v>142</v>
       </c>
@@ -4613,7 +4642,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>143</v>
       </c>
@@ -4624,7 +4653,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>144</v>
       </c>
@@ -4635,7 +4664,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>145</v>
       </c>
@@ -4646,7 +4675,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
         <v>146</v>
       </c>
@@ -4657,7 +4686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>147</v>
       </c>
@@ -4668,7 +4697,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
         <v>148</v>
       </c>
@@ -4679,7 +4708,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>149</v>
       </c>
@@ -4690,7 +4719,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="32" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>150</v>
       </c>
@@ -4701,7 +4730,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
         <v>151</v>
       </c>
@@ -4712,7 +4741,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="30" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
         <v>152</v>
       </c>
@@ -4723,7 +4752,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
         <v>153</v>
       </c>
@@ -4734,7 +4763,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>154</v>
       </c>
@@ -4745,7 +4774,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>155</v>
       </c>
@@ -4756,7 +4785,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>156</v>
       </c>
@@ -4767,7 +4796,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
         <v>157</v>
       </c>
@@ -4778,7 +4807,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>158</v>
       </c>
@@ -4789,7 +4818,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="42" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A44" s="42" t="s">
         <v>212</v>
       </c>
@@ -4800,7 +4829,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
         <v>213</v>
       </c>
@@ -4811,7 +4840,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
         <v>214</v>
       </c>
@@ -4822,7 +4851,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="46" t="s">
         <v>227</v>
       </c>
@@ -4833,7 +4862,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="46" t="s">
         <v>228</v>
       </c>
@@ -4844,7 +4873,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="46" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
Updated xlsx file for the Sprint 2
</commit_message>
<xml_diff>
--- a/TeamDhruvAnuragDishantDeeptiReport.xlsx
+++ b/TeamDhruvAnuragDishantDeeptiReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepti.agrawal\github\CS_555_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dishantnaik/Documents/MS/Semester_3/SSW 555/Project/CS_555_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA1DE3F-5DE9-4FC4-BF7F-0B3245274631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EF4EF4-36D0-E94B-A5C8-DDA63AEDADC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="242">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1247,7 +1247,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1318,7 +1318,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2305,16 +2305,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="13" customWidth="1"/>
     <col min="4" max="5" width="20.5" style="13" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="22" t="s">
         <v>197</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="24" t="s">
         <v>198</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>199</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
         <v>200</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="39" t="s">
         <v>207</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="47" t="s">
         <v>222</v>
       </c>
@@ -2433,8 +2433,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D9" s="41" t="s">
         <v>34</v>
       </c>
@@ -2469,20 +2469,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="6.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="22" t="s">
         <v>144</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" s="22" t="s">
         <v>149</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>2</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>2</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" s="22" t="s">
         <v>154</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>1</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" s="24" t="s">
         <v>119</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" s="24" t="s">
         <v>122</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" s="24" t="s">
         <v>123</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" s="24" t="s">
         <v>133</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" s="24" t="s">
         <v>137</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B17" s="24" t="s">
         <v>141</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>1</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>1</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B20" s="28" t="s">
         <v>131</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B21" s="28" t="s">
         <v>132</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" s="28" t="s">
         <v>139</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B23" s="28" t="s">
         <v>143</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B24" s="28" t="s">
         <v>150</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" s="28" t="s">
         <v>156</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" s="26" t="s">
         <v>124</v>
       </c>
@@ -2876,7 +2876,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="13">
+        <v>2</v>
+      </c>
       <c r="B27" s="26" t="s">
         <v>125</v>
       </c>
@@ -2887,10 +2890,10 @@
         <v>199</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>1</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B29" s="26" t="s">
         <v>130</v>
       </c>
@@ -2921,7 +2924,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A30" s="13">
+        <v>2</v>
+      </c>
       <c r="B30" s="26" t="s">
         <v>138</v>
       </c>
@@ -2932,10 +2938,10 @@
         <v>199</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B31" s="26" t="s">
         <v>148</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>1</v>
       </c>
@@ -2966,7 +2972,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" s="26" t="s">
         <v>158</v>
       </c>
@@ -2980,7 +2986,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" s="39" t="s">
         <v>127</v>
       </c>
@@ -2994,7 +3000,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" s="39" t="s">
         <v>128</v>
       </c>
@@ -3008,7 +3014,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="13">
         <v>1</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B37" s="39" t="s">
         <v>134</v>
       </c>
@@ -3039,7 +3045,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B38" s="39" t="s">
         <v>135</v>
       </c>
@@ -3053,7 +3059,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B39" s="39" t="s">
         <v>212</v>
       </c>
@@ -3067,7 +3073,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="13">
         <v>1</v>
       </c>
@@ -3084,7 +3090,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" s="39" t="s">
         <v>214</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B42" s="47" t="s">
         <v>136</v>
       </c>
@@ -3112,7 +3118,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" s="47" t="s">
         <v>140</v>
       </c>
@@ -3126,7 +3132,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B44" s="47" t="s">
         <v>142</v>
       </c>
@@ -3140,7 +3146,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B45" s="47" t="s">
         <v>153</v>
       </c>
@@ -3154,7 +3160,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B46" s="47" t="s">
         <v>157</v>
       </c>
@@ -3168,7 +3174,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="13">
         <v>1</v>
       </c>
@@ -3185,7 +3191,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B48" s="47" t="s">
         <v>228</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="13">
         <v>1</v>
       </c>
@@ -3216,7 +3222,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B50" s="51"/>
     </row>
   </sheetData>
@@ -3236,50 +3242,50 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="6"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>164</v>
       </c>
@@ -3302,7 +3308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -3318,7 +3324,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>166</v>
       </c>
@@ -3343,7 +3349,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>167</v>
       </c>
@@ -3368,7 +3374,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>168</v>
       </c>
@@ -3393,7 +3399,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>169</v>
       </c>
@@ -3433,16 +3439,16 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3462,7 +3468,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="17">
         <v>42633</v>
       </c>
@@ -3476,7 +3482,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="17">
         <v>42657</v>
       </c>
@@ -3486,7 +3492,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="17">
         <v>42683</v>
       </c>
@@ -3496,7 +3502,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="17">
         <v>42708</v>
       </c>
@@ -3506,7 +3512,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="17">
         <v>42728</v>
       </c>
@@ -3532,21 +3538,21 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="27.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="13" customWidth="1"/>
     <col min="4" max="4" width="11" style="13"/>
-    <col min="5" max="5" width="6.875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="13" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="13" customWidth="1"/>
-    <col min="7" max="7" width="6.625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -3575,7 +3581,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>146</v>
       </c>
@@ -3633,7 +3639,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
         <v>147</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>117</v>
       </c>
@@ -3691,7 +3697,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>118</v>
       </c>
@@ -3720,7 +3726,7 @@
         <v>42646</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
         <v>126</v>
       </c>
@@ -3749,7 +3755,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
         <v>155</v>
       </c>
@@ -3778,7 +3784,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -3807,7 +3813,7 @@
         <v>42644</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -3836,7 +3842,7 @@
         <v>42639</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
         <v>213</v>
       </c>
@@ -3865,7 +3871,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
         <v>129</v>
       </c>
@@ -3894,7 +3900,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
         <v>227</v>
       </c>
@@ -3923,7 +3929,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="13" t="s">
         <v>229</v>
       </c>
@@ -3952,35 +3958,35 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B16" s="19"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="14" t="s">
         <v>36</v>
       </c>
@@ -3997,12 +4003,12 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -4031,7 +4037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>151</v>
       </c>
@@ -4054,7 +4060,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
         <v>152</v>
       </c>
@@ -4077,29 +4083,53 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="13">
+        <v>60</v>
+      </c>
+      <c r="F4" s="13">
+        <v>90</v>
+      </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="13">
+        <v>40</v>
+      </c>
+      <c r="F5" s="13">
+        <v>90</v>
+      </c>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4110,7 +4140,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4121,7 +4151,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4132,7 +4162,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4158,9 +4188,9 @@
       <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4189,7 +4219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -4200,7 +4230,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -4211,7 +4241,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -4222,7 +4252,7 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -4233,7 +4263,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -4244,7 +4274,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -4255,7 +4285,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -4266,7 +4296,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -4291,12 +4321,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="11" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -4335,17 +4365,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>116</v>
       </c>
@@ -4356,7 +4386,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
         <v>117</v>
       </c>
@@ -4367,7 +4397,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="34" t="s">
         <v>118</v>
       </c>
@@ -4378,7 +4408,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="34" t="s">
         <v>119</v>
       </c>
@@ -4389,7 +4419,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
         <v>120</v>
       </c>
@@ -4400,7 +4430,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
         <v>121</v>
       </c>
@@ -4411,7 +4441,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="34" t="s">
         <v>122</v>
       </c>
@@ -4422,7 +4452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="34" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="34" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="34" t="s">
         <v>123</v>
       </c>
@@ -4433,7 +4463,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="36" t="s">
         <v>124</v>
       </c>
@@ -4444,7 +4474,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="36" t="s">
         <v>125</v>
       </c>
@@ -4455,7 +4485,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="36" t="s">
         <v>126</v>
       </c>
@@ -4466,7 +4496,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" s="42" t="s">
         <v>127</v>
       </c>
@@ -4477,7 +4507,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="42" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="42" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" s="42" t="s">
         <v>128</v>
       </c>
@@ -4488,7 +4518,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="42" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="42" customFormat="1" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" s="42" t="s">
         <v>129</v>
       </c>
@@ -4499,7 +4529,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" s="36" t="s">
         <v>130</v>
       </c>
@@ -4510,7 +4540,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
         <v>131</v>
       </c>
@@ -4521,7 +4551,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
@@ -4532,7 +4562,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="34" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="34" t="s">
         <v>133</v>
       </c>
@@ -4543,7 +4573,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="42" t="s">
         <v>134</v>
       </c>
@@ -4554,7 +4584,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="42" t="s">
         <v>135</v>
       </c>
@@ -4565,7 +4595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" s="44" t="s">
         <v>136</v>
       </c>
@@ -4576,7 +4606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" s="34" t="s">
         <v>137</v>
       </c>
@@ -4587,7 +4617,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" s="36" t="s">
         <v>138</v>
       </c>
@@ -4598,7 +4628,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
         <v>139</v>
       </c>
@@ -4609,7 +4639,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="44" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" s="44" t="s">
         <v>140</v>
       </c>
@@ -4620,7 +4650,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="34" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" s="34" t="s">
         <v>141</v>
       </c>
@@ -4631,7 +4661,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="44" customFormat="1" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="44" customFormat="1" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" s="44" t="s">
         <v>142</v>
       </c>
@@ -4642,7 +4672,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" s="32" t="s">
         <v>143</v>
       </c>
@@ -4653,7 +4683,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" s="30" t="s">
         <v>144</v>
       </c>
@@ -4664,7 +4694,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="30" t="s">
         <v>145</v>
       </c>
@@ -4675,7 +4705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="30" t="s">
         <v>146</v>
       </c>
@@ -4686,7 +4716,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" s="30" t="s">
         <v>147</v>
       </c>
@@ -4697,7 +4727,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="36" t="s">
         <v>148</v>
       </c>
@@ -4708,7 +4738,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" s="30" t="s">
         <v>149</v>
       </c>
@@ -4719,7 +4749,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="32" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="32" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" s="32" t="s">
         <v>150</v>
       </c>
@@ -4730,7 +4760,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="30" t="s">
         <v>151</v>
       </c>
@@ -4741,7 +4771,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" s="30" t="s">
         <v>152</v>
       </c>
@@ -4752,7 +4782,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" s="44" t="s">
         <v>153</v>
       </c>
@@ -4763,7 +4793,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="30" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" s="30" t="s">
         <v>154</v>
       </c>
@@ -4774,7 +4804,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" s="36" t="s">
         <v>155</v>
       </c>
@@ -4785,7 +4815,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="32" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="32" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" s="32" t="s">
         <v>156</v>
       </c>
@@ -4796,7 +4826,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="44" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" s="44" t="s">
         <v>157</v>
       </c>
@@ -4807,7 +4837,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="36" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="36" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" s="36" t="s">
         <v>158</v>
       </c>
@@ -4818,7 +4848,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" s="42" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A44" s="42" t="s">
         <v>212</v>
       </c>
@@ -4829,7 +4859,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A45" s="42" t="s">
         <v>213</v>
       </c>
@@ -4840,7 +4870,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="42" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="42" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A46" s="42" t="s">
         <v>214</v>
       </c>
@@ -4851,7 +4881,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A47" s="46" t="s">
         <v>227</v>
       </c>
@@ -4862,7 +4892,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="46" t="s">
         <v>228</v>
       </c>
@@ -4873,7 +4903,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="44" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="44" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A49" s="46" t="s">
         <v>229</v>
       </c>

</xml_diff>